<commit_message>
1.3 code cleanup, load data from object, json, url (json)
</commit_message>
<xml_diff>
--- a/Test/Test1.xlsx
+++ b/Test/Test1.xlsx
@@ -47,7 +47,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="238"/>
           </rPr>
           <t>Marcin Kotynia:</t>
         </r>
@@ -56,7 +57,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="238"/>
           </rPr>
           <t xml:space="preserve">
 Hello World 
@@ -69,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="168">
   <si>
     <t>Alligned Left</t>
   </si>
@@ -564,6 +566,15 @@
   </si>
   <si>
     <t>Cell With A comment</t>
+  </si>
+  <si>
+    <t>[[d[0][!].Category]]</t>
+  </si>
+  <si>
+    <t>[[d[0][!].arrest_count]]</t>
+  </si>
+  <si>
+    <t>Crime Statistics from http://nflarrest.com/api/v1/crime</t>
   </si>
 </sst>
 </file>
@@ -663,14 +674,16 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="74">
@@ -1209,7 +1222,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
+      <left style="thin">
         <color theme="5"/>
       </left>
       <right style="thick">
@@ -1218,7 +1231,7 @@
       <top style="thick">
         <color theme="5"/>
       </top>
-      <bottom style="thick">
+      <bottom style="medium">
         <color theme="5"/>
       </bottom>
       <diagonal/>
@@ -1332,7 +1345,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1348,6 +1360,7 @@
     <xf numFmtId="0" fontId="0" fillId="71" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="72" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="73" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
@@ -1444,6 +1457,471 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>225144</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>70208</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Person icon" descr="&quot;&quot;" title="Person icon">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E721D013-DA28-4E5D-BC6F-39C2D5F41CEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6858000" y="5629275"/>
+          <a:ext cx="225144" cy="317858"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="T0" fmla="*/ 209 w 376"/>
+            <a:gd name="T1" fmla="*/ 3 h 523"/>
+            <a:gd name="T2" fmla="*/ 248 w 376"/>
+            <a:gd name="T3" fmla="*/ 21 h 523"/>
+            <a:gd name="T4" fmla="*/ 274 w 376"/>
+            <a:gd name="T5" fmla="*/ 55 h 523"/>
+            <a:gd name="T6" fmla="*/ 285 w 376"/>
+            <a:gd name="T7" fmla="*/ 97 h 523"/>
+            <a:gd name="T8" fmla="*/ 295 w 376"/>
+            <a:gd name="T9" fmla="*/ 122 h 523"/>
+            <a:gd name="T10" fmla="*/ 305 w 376"/>
+            <a:gd name="T11" fmla="*/ 139 h 523"/>
+            <a:gd name="T12" fmla="*/ 302 w 376"/>
+            <a:gd name="T13" fmla="*/ 161 h 523"/>
+            <a:gd name="T14" fmla="*/ 285 w 376"/>
+            <a:gd name="T15" fmla="*/ 172 h 523"/>
+            <a:gd name="T16" fmla="*/ 282 w 376"/>
+            <a:gd name="T17" fmla="*/ 198 h 523"/>
+            <a:gd name="T18" fmla="*/ 260 w 376"/>
+            <a:gd name="T19" fmla="*/ 239 h 523"/>
+            <a:gd name="T20" fmla="*/ 223 w 376"/>
+            <a:gd name="T21" fmla="*/ 265 h 523"/>
+            <a:gd name="T22" fmla="*/ 240 w 376"/>
+            <a:gd name="T23" fmla="*/ 267 h 523"/>
+            <a:gd name="T24" fmla="*/ 246 w 376"/>
+            <a:gd name="T25" fmla="*/ 268 h 523"/>
+            <a:gd name="T26" fmla="*/ 341 w 376"/>
+            <a:gd name="T27" fmla="*/ 292 h 523"/>
+            <a:gd name="T28" fmla="*/ 366 w 376"/>
+            <a:gd name="T29" fmla="*/ 316 h 523"/>
+            <a:gd name="T30" fmla="*/ 376 w 376"/>
+            <a:gd name="T31" fmla="*/ 351 h 523"/>
+            <a:gd name="T32" fmla="*/ 374 w 376"/>
+            <a:gd name="T33" fmla="*/ 509 h 523"/>
+            <a:gd name="T34" fmla="*/ 362 w 376"/>
+            <a:gd name="T35" fmla="*/ 521 h 523"/>
+            <a:gd name="T36" fmla="*/ 23 w 376"/>
+            <a:gd name="T37" fmla="*/ 523 h 523"/>
+            <a:gd name="T38" fmla="*/ 6 w 376"/>
+            <a:gd name="T39" fmla="*/ 516 h 523"/>
+            <a:gd name="T40" fmla="*/ 0 w 376"/>
+            <a:gd name="T41" fmla="*/ 500 h 523"/>
+            <a:gd name="T42" fmla="*/ 2 w 376"/>
+            <a:gd name="T43" fmla="*/ 332 h 523"/>
+            <a:gd name="T44" fmla="*/ 20 w 376"/>
+            <a:gd name="T45" fmla="*/ 302 h 523"/>
+            <a:gd name="T46" fmla="*/ 52 w 376"/>
+            <a:gd name="T47" fmla="*/ 285 h 523"/>
+            <a:gd name="T48" fmla="*/ 132 w 376"/>
+            <a:gd name="T49" fmla="*/ 268 h 523"/>
+            <a:gd name="T50" fmla="*/ 152 w 376"/>
+            <a:gd name="T51" fmla="*/ 265 h 523"/>
+            <a:gd name="T52" fmla="*/ 115 w 376"/>
+            <a:gd name="T53" fmla="*/ 240 h 523"/>
+            <a:gd name="T54" fmla="*/ 93 w 376"/>
+            <a:gd name="T55" fmla="*/ 198 h 523"/>
+            <a:gd name="T56" fmla="*/ 90 w 376"/>
+            <a:gd name="T57" fmla="*/ 172 h 523"/>
+            <a:gd name="T58" fmla="*/ 73 w 376"/>
+            <a:gd name="T59" fmla="*/ 161 h 523"/>
+            <a:gd name="T60" fmla="*/ 70 w 376"/>
+            <a:gd name="T61" fmla="*/ 139 h 523"/>
+            <a:gd name="T62" fmla="*/ 80 w 376"/>
+            <a:gd name="T63" fmla="*/ 122 h 523"/>
+            <a:gd name="T64" fmla="*/ 90 w 376"/>
+            <a:gd name="T65" fmla="*/ 97 h 523"/>
+            <a:gd name="T66" fmla="*/ 99 w 376"/>
+            <a:gd name="T67" fmla="*/ 55 h 523"/>
+            <a:gd name="T68" fmla="*/ 126 w 376"/>
+            <a:gd name="T69" fmla="*/ 21 h 523"/>
+            <a:gd name="T70" fmla="*/ 165 w 376"/>
+            <a:gd name="T71" fmla="*/ 3 h 523"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="T0" y="T1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T2" y="T3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T4" y="T5"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T6" y="T7"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T8" y="T9"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T10" y="T11"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T12" y="T13"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T14" y="T15"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T16" y="T17"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T18" y="T19"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T20" y="T21"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T22" y="T23"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T24" y="T25"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T26" y="T27"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T28" y="T29"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T30" y="T31"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T32" y="T33"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T34" y="T35"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T36" y="T37"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T38" y="T39"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T40" y="T41"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T42" y="T43"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T44" y="T45"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T46" y="T47"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T48" y="T49"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T50" y="T51"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T52" y="T53"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T54" y="T55"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T56" y="T57"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T58" y="T59"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T60" y="T61"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T62" y="T63"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T64" y="T65"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T66" y="T67"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T68" y="T69"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="T70" y="T71"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="376" h="523">
+              <a:moveTo>
+                <a:pt x="187" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="209" y="3"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="230" y="10"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="248" y="21"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="263" y="36"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="274" y="55"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="282" y="75"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="285" y="97"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="285" y="120"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="295" y="122"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="302" y="129"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="305" y="139"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="305" y="151"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="302" y="161"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="295" y="169"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="285" y="172"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="285" y="175"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="282" y="198"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="273" y="220"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="260" y="239"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="243" y="254"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="223" y="265"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="232" y="266"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="240" y="267"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="245" y="268"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="246" y="268"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="323" y="285"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="341" y="292"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="355" y="302"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="366" y="316"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="373" y="332"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="376" y="351"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="376" y="500"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="374" y="509"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="369" y="516"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="362" y="521"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="353" y="523"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="23" y="523"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="14" y="521"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="6" y="516"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1" y="509"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="500"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="351"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="2" y="332"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="9" y="316"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="20" y="302"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="35" y="292"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="52" y="285"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="129" y="268"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="132" y="268"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="140" y="267"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="152" y="265"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="132" y="255"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="115" y="240"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="101" y="220"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="93" y="198"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="90" y="175"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="90" y="172"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="80" y="169"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="73" y="161"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="70" y="151"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="70" y="139"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="73" y="129"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="80" y="122"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="90" y="120"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="90" y="97"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="92" y="75"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="99" y="55"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="112" y="36"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="126" y="21"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="144" y="10"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="165" y="3"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="187" y="0"/>
+              </a:lnTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1763,8 +2241,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:S59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U28" sqref="U28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1772,6 +2250,7 @@
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
     <col min="7" max="7" width="5.5703125" customWidth="1"/>
     <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.5703125" customWidth="1"/>
@@ -1869,7 +2348,7 @@
       <c r="C3" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="78" t="s">
+      <c r="D3" s="77" t="s">
         <v>115</v>
       </c>
       <c r="I3" s="7" t="s">
@@ -1885,7 +2364,7 @@
         <f>K3+L3</f>
         <v>3</v>
       </c>
-      <c r="N3" s="74" t="s">
+      <c r="N3" s="73" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1963,7 +2442,7 @@
         <v>122</v>
       </c>
       <c r="M7" s="2"/>
-      <c r="Q7" s="80" t="s">
+      <c r="Q7" s="79" t="s">
         <v>154</v>
       </c>
     </row>
@@ -1985,7 +2464,7 @@
       <c r="G8" s="90"/>
       <c r="H8" s="69"/>
       <c r="M8" s="2"/>
-      <c r="Q8" s="79" t="s">
+      <c r="Q8" s="78" t="s">
         <v>156</v>
       </c>
     </row>
@@ -2006,7 +2485,7 @@
         <v>123</v>
       </c>
       <c r="M9" s="2"/>
-      <c r="Q9" s="81" t="s">
+      <c r="Q9" s="80" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2024,7 +2503,7 @@
         <v>1</v>
       </c>
       <c r="M10" s="2"/>
-      <c r="Q10" s="84" t="s">
+      <c r="Q10" s="83" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2042,7 +2521,7 @@
         <v>2</v>
       </c>
       <c r="M11" s="2"/>
-      <c r="Q11" s="82" t="s">
+      <c r="Q11" s="81" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2059,15 +2538,15 @@
       <c r="D12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I12" s="73" t="s">
+      <c r="I12" s="88" t="s">
         <v>124</v>
       </c>
       <c r="M12" s="2"/>
-      <c r="Q12" s="83" t="s">
+      <c r="Q12" s="82" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
@@ -2081,7 +2560,7 @@
         <v>7</v>
       </c>
       <c r="M13" s="2"/>
-      <c r="Q13" s="85" t="s">
+      <c r="Q13" s="84" t="s">
         <v>160</v>
       </c>
     </row>
@@ -2098,11 +2577,11 @@
       <c r="D14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I14" s="75" t="s">
+      <c r="I14" s="74" t="s">
         <v>130</v>
       </c>
       <c r="M14" s="2"/>
-      <c r="Q14" s="86" t="s">
+      <c r="Q14" s="85" t="s">
         <v>161</v>
       </c>
     </row>
@@ -2120,7 +2599,7 @@
         <v>4</v>
       </c>
       <c r="M15" s="2"/>
-      <c r="Q15" s="87" t="s">
+      <c r="Q15" s="86" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2137,11 +2616,11 @@
       <c r="D16" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I16" s="76" t="s">
+      <c r="I16" s="75" t="s">
         <v>131</v>
       </c>
       <c r="M16" s="2"/>
-      <c r="Q16" s="88" t="s">
+      <c r="Q16" s="87" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2173,7 +2652,7 @@
       <c r="D18" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I18" s="77" t="s">
+      <c r="I18" s="76" t="s">
         <v>132</v>
       </c>
       <c r="M18" s="2"/>
@@ -2253,6 +2732,16 @@
       <c r="C24" t="s">
         <v>88</v>
       </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <f>E24+F24</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="25" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -2264,6 +2753,13 @@
       <c r="C25" t="s">
         <v>89</v>
       </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <f>E25+F25</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="26" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -2275,6 +2771,10 @@
       <c r="C26" t="s">
         <v>90</v>
       </c>
+      <c r="G26">
+        <f>SUM(G23:G25)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="27" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -2297,6 +2797,9 @@
       <c r="C28" t="s">
         <v>78</v>
       </c>
+      <c r="D28" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="29" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29">
@@ -2307,6 +2810,12 @@
       </c>
       <c r="C29" t="s">
         <v>74</v>
+      </c>
+      <c r="D29" t="s">
+        <v>165</v>
+      </c>
+      <c r="E29" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2645,6 +3154,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>